<commit_message>
played with nominatons they need to be added to extended df
</commit_message>
<xml_diff>
--- a/viz/nom_win.xlsx
+++ b/viz/nom_win.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksandra Czaplak\Desktop\oscars_ml\oscar_predictions\viz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B193B8E-656B-42CC-BBB9-6BAD6BC1E39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7B6E22-8660-4677-BEB4-1405CB5BDEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
+    <workbookView xWindow="338" yWindow="3060" windowWidth="13680" windowHeight="8085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nom_win" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -139,9 +140,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -656,10 +657,10 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1024,7 +1025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>